<commit_message>
more python program addded
</commit_message>
<xml_diff>
--- a/Python_Positive and Negative Indexing.xlsx
+++ b/Python_Positive and Negative Indexing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suni Admin\Desktop\data-science-training\PythonCoLab0908_Suniti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{717086E6-5C6E-42E6-AF89-ECADD5A8FB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA58693-2E1C-4B86-9A8F-0DEC6DB7032A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="-2604" windowWidth="23232" windowHeight="12432" xr2:uid="{E9164621-1558-404A-9649-CDBBF3FE5FCE}"/>
+    <workbookView xWindow="24006" yWindow="-2508" windowWidth="14472" windowHeight="12318" xr2:uid="{E9164621-1558-404A-9649-CDBBF3FE5FCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
     <t>Position</t>
   </si>
@@ -96,6 +96,81 @@
   </si>
   <si>
     <t>Fourth</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>cherry</t>
+  </si>
+  <si>
+    <t>dates</t>
+  </si>
+  <si>
+    <t>eggfruit</t>
+  </si>
+  <si>
+    <t>fig</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
   </si>
 </sst>
 </file>
@@ -125,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,15 +208,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00858BF7-E017-4669-A926-32F5EAE09F42}">
-  <dimension ref="A2:L21"/>
+  <dimension ref="A2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -612,12 +709,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>16</v>
       </c>
@@ -631,7 +728,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -651,7 +748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>13</v>
       </c>
@@ -667,6 +764,566 @@
       <c r="F21">
         <v>-1</v>
       </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25" s="5">
+        <v>3</v>
+      </c>
+      <c r="F25" s="5">
+        <v>4</v>
+      </c>
+      <c r="G25" s="5">
+        <v>5</v>
+      </c>
+      <c r="H25" s="5">
+        <v>6</v>
+      </c>
+      <c r="I25" s="5">
+        <v>7</v>
+      </c>
+      <c r="J25" s="5">
+        <v>8</v>
+      </c>
+      <c r="K25" s="5">
+        <v>9</v>
+      </c>
+      <c r="L25" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
+        <v>2</v>
+      </c>
+      <c r="F27" s="5">
+        <v>3</v>
+      </c>
+      <c r="G27" s="5">
+        <v>4</v>
+      </c>
+      <c r="H27" s="5">
+        <v>5</v>
+      </c>
+      <c r="I27" s="5">
+        <v>6</v>
+      </c>
+      <c r="J27" s="5">
+        <v>7</v>
+      </c>
+      <c r="K27" s="5">
+        <v>8</v>
+      </c>
+      <c r="L27" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D28" s="5">
+        <v>-9</v>
+      </c>
+      <c r="E28" s="5">
+        <v>-8</v>
+      </c>
+      <c r="F28" s="5">
+        <v>-7</v>
+      </c>
+      <c r="G28" s="5">
+        <v>-6</v>
+      </c>
+      <c r="H28" s="5">
+        <v>-5</v>
+      </c>
+      <c r="I28" s="5">
+        <v>-4</v>
+      </c>
+      <c r="J28" s="5">
+        <v>-3</v>
+      </c>
+      <c r="K28" s="5">
+        <v>-2</v>
+      </c>
+      <c r="L28" s="5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5">
+        <v>3</v>
+      </c>
+      <c r="F31" s="5">
+        <v>4</v>
+      </c>
+      <c r="G31" s="5">
+        <v>5</v>
+      </c>
+      <c r="H31" s="5">
+        <v>6</v>
+      </c>
+      <c r="I31" s="5">
+        <v>7</v>
+      </c>
+      <c r="J31" s="5">
+        <v>8</v>
+      </c>
+      <c r="K31" s="5">
+        <v>9</v>
+      </c>
+      <c r="L31" s="5">
+        <v>10</v>
+      </c>
+      <c r="M31" s="6">
+        <v>11</v>
+      </c>
+      <c r="N31" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="5">
+        <v>0</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5">
+        <v>2</v>
+      </c>
+      <c r="F33" s="5">
+        <v>3</v>
+      </c>
+      <c r="G33" s="5">
+        <v>4</v>
+      </c>
+      <c r="H33" s="5">
+        <v>5</v>
+      </c>
+      <c r="I33" s="5">
+        <v>6</v>
+      </c>
+      <c r="J33" s="5">
+        <v>7</v>
+      </c>
+      <c r="K33" s="5">
+        <v>8</v>
+      </c>
+      <c r="L33" s="5">
+        <v>9</v>
+      </c>
+      <c r="M33" s="6">
+        <v>10</v>
+      </c>
+      <c r="N33" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="6">
+        <v>-12</v>
+      </c>
+      <c r="D34" s="6">
+        <v>-11</v>
+      </c>
+      <c r="E34" s="6">
+        <v>-10</v>
+      </c>
+      <c r="F34" s="6">
+        <v>-9</v>
+      </c>
+      <c r="G34" s="6">
+        <v>-8</v>
+      </c>
+      <c r="H34" s="6">
+        <v>-7</v>
+      </c>
+      <c r="I34" s="6">
+        <v>-6</v>
+      </c>
+      <c r="J34" s="6">
+        <v>-5</v>
+      </c>
+      <c r="K34" s="6">
+        <v>-4</v>
+      </c>
+      <c r="L34" s="6">
+        <v>-3</v>
+      </c>
+      <c r="M34" s="6">
+        <v>-2</v>
+      </c>
+      <c r="N34" s="6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5">
+        <v>3</v>
+      </c>
+      <c r="F37" s="5">
+        <v>4</v>
+      </c>
+      <c r="G37" s="5">
+        <v>5</v>
+      </c>
+      <c r="H37" s="5">
+        <v>6</v>
+      </c>
+      <c r="I37" s="5">
+        <v>7</v>
+      </c>
+      <c r="J37" s="5">
+        <v>8</v>
+      </c>
+      <c r="K37" s="5">
+        <v>9</v>
+      </c>
+      <c r="L37" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5">
+        <v>2</v>
+      </c>
+      <c r="F39" s="5">
+        <v>3</v>
+      </c>
+      <c r="G39" s="5">
+        <v>4</v>
+      </c>
+      <c r="H39" s="5">
+        <v>5</v>
+      </c>
+      <c r="I39" s="5">
+        <v>6</v>
+      </c>
+      <c r="J39" s="5">
+        <v>7</v>
+      </c>
+      <c r="K39" s="5">
+        <v>8</v>
+      </c>
+      <c r="L39" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D40" s="5">
+        <v>-9</v>
+      </c>
+      <c r="E40" s="5">
+        <v>-8</v>
+      </c>
+      <c r="F40" s="5">
+        <v>-7</v>
+      </c>
+      <c r="G40" s="5">
+        <v>-6</v>
+      </c>
+      <c r="H40" s="5">
+        <v>-5</v>
+      </c>
+      <c r="I40" s="5">
+        <v>-4</v>
+      </c>
+      <c r="J40" s="5">
+        <v>-3</v>
+      </c>
+      <c r="K40" s="5">
+        <v>-2</v>
+      </c>
+      <c r="L40" s="5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5">
+        <v>1</v>
+      </c>
+      <c r="D43" s="5">
+        <v>2</v>
+      </c>
+      <c r="E43" s="5">
+        <v>3</v>
+      </c>
+      <c r="F43" s="5">
+        <v>4</v>
+      </c>
+      <c r="G43" s="5">
+        <v>5</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="5">
+        <v>0</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5">
+        <v>2</v>
+      </c>
+      <c r="F45" s="5">
+        <v>3</v>
+      </c>
+      <c r="G45" s="5">
+        <v>4</v>
+      </c>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="5">
+        <v>-5</v>
+      </c>
+      <c r="D46" s="5">
+        <v>-4</v>
+      </c>
+      <c r="E46" s="5">
+        <v>-3</v>
+      </c>
+      <c r="F46" s="5">
+        <v>-2</v>
+      </c>
+      <c r="G46" s="5">
+        <v>-1</v>
+      </c>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>